<commit_message>
fix & add ContractPause
</commit_message>
<xml_diff>
--- a/FunctionCheck.xlsx
+++ b/FunctionCheck.xlsx
@@ -9,7 +9,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zy/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:10001_{0CDB3ACB-BDD3-144B-99B4-433A3F5173BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:10001_{9FE40E98-C5FF-3F48-904A-B46E4FDE6ED0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19300" yWindow="500" windowWidth="31900" windowHeight="25940" xr2:uid="{E34BA6AF-FC0C-A84B-B30E-63378FD07636}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="(old)功能设计_20240714" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">功能设计_20241016!$A$2:$P$28</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">功能设计_20241016!$A$2:$P$30</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="209">
   <si>
     <t>Caller</t>
     <phoneticPr fontId="1"/>
@@ -5201,10 +5201,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>checkChangeCreationCreator</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="12"/>
@@ -5420,6 +5416,300 @@
   <si>
     <t>uint256 pointBalance
 uint256 blockTimeStamp</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>changeContractPausedStatus</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>checkChangeContractPausedStatus</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>（预检）暂停积</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>分</t>
+    </r>
+    <rPh sb="0" eb="1">
+      <t>ji fen</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>zan ting</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>预处</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>理</t>
+    </r>
+    <rPh sb="0" eb="1">
+      <t>yu chu li</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">address
+contractAddress
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>对</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>象合</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>约</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>地址</t>
+    </r>
+    <rPh sb="24" eb="25">
+      <t>dui xiang</t>
+    </rPh>
+    <rPh sb="26" eb="27">
+      <t>he yue</t>
+    </rPh>
+    <rPh sb="28" eb="29">
+      <t>di zhi</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>address
+senderAddress
+必</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="2"/>
+        <charset val="128"/>
+      </rPr>
+      <t>须</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>是creator</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>暂停积</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>分</t>
+    </r>
+    <rPh sb="0" eb="1">
+      <t>zan ting</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>执</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>行</t>
+    </r>
+    <rPh sb="0" eb="1">
+      <t>zhi xing</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>uint256 feeAmount
+(支付平台手</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>续费额</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>度)</t>
+    </r>
+    <rPh sb="19" eb="20">
+      <t>zhi fu de</t>
+    </rPh>
+    <rPh sb="21" eb="22">
+      <t>ping tai shou xu</t>
+    </rPh>
+    <rPh sb="27" eb="28">
+      <t>du</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>checkChangeCreationCreator</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t xml:space="preserve">
+checkChangeContractCreator</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>changeCreationCreator</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t xml:space="preserve">
+changeContractCreator</t>
+    </r>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -5427,7 +5717,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="16">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -5492,6 +5782,60 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="游ゴシック"/>
+      <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="游ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="游ゴシック"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Microsoft YaHei"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Microsoft YaHei"/>
+      <family val="2"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="游ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="游ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -5515,7 +5859,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -5568,16 +5912,37 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5608,8 +5973,8 @@
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>183444</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>225624</xdr:rowOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>140957</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6011,11 +6376,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBA4FD5B-D9BE-9A41-89B1-9B1F95EF810F}">
-  <dimension ref="A1:P36"/>
+  <dimension ref="A1:P38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M13" sqref="M13"/>
+      <pane ySplit="2" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -6035,34 +6400,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18" t="s">
+      <c r="C1" s="17"/>
+      <c r="D1" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18" t="s">
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:16">
-      <c r="A2" s="19"/>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
+      <c r="A2" s="18"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
       <c r="D2" t="s">
         <v>0</v>
       </c>
@@ -6093,7 +6458,7 @@
       <c r="N2" t="s">
         <v>22</v>
       </c>
-      <c r="O2" s="19"/>
+      <c r="O2" s="18"/>
     </row>
     <row r="3" spans="1:16" ht="42">
       <c r="B3" s="20" t="s">
@@ -6161,7 +6526,7 @@
       <c r="O4" s="3"/>
     </row>
     <row r="5" spans="1:16" ht="63">
-      <c r="B5" s="19"/>
+      <c r="B5" s="18"/>
       <c r="C5" s="14" t="s">
         <v>56</v>
       </c>
@@ -6191,7 +6556,7 @@
       <c r="O5" s="3"/>
     </row>
     <row r="6" spans="1:16" ht="42">
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="19" t="s">
         <v>164</v>
       </c>
       <c r="C6" s="13" t="s">
@@ -6397,7 +6762,7 @@
       <c r="O11" s="3"/>
     </row>
     <row r="12" spans="1:16" ht="84">
-      <c r="B12" s="17"/>
+      <c r="B12" s="19"/>
       <c r="C12" s="13" t="s">
         <v>166</v>
       </c>
@@ -6437,7 +6802,7 @@
       </c>
     </row>
     <row r="13" spans="1:16" ht="63">
-      <c r="B13" s="19"/>
+      <c r="B13" s="18"/>
       <c r="C13" s="13" t="s">
         <v>135</v>
       </c>
@@ -6469,7 +6834,7 @@
       <c r="O13" s="3"/>
     </row>
     <row r="14" spans="1:16" ht="63">
-      <c r="B14" s="19"/>
+      <c r="B14" s="18"/>
       <c r="C14" s="13" t="s">
         <v>148</v>
       </c>
@@ -6501,7 +6866,7 @@
       <c r="O14" s="3"/>
     </row>
     <row r="15" spans="1:16" ht="42">
-      <c r="B15" s="19"/>
+      <c r="B15" s="18"/>
       <c r="C15" s="13" t="s">
         <v>136</v>
       </c>
@@ -6533,7 +6898,7 @@
       <c r="O15" s="3"/>
     </row>
     <row r="16" spans="1:16" ht="63">
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="19" t="s">
         <v>95</v>
       </c>
       <c r="C16" s="15" t="s">
@@ -6560,13 +6925,13 @@
       <c r="J16" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K16" s="3" t="s">
+      <c r="K16" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="L16" s="3" t="s">
+      <c r="L16" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="M16" s="3" t="s">
+      <c r="M16" s="22" t="s">
         <v>178</v>
       </c>
       <c r="N16" s="3"/>
@@ -6574,7 +6939,7 @@
       <c r="P16" s="3"/>
     </row>
     <row r="17" spans="2:16" ht="63">
-      <c r="B17" s="17"/>
+      <c r="B17" s="19"/>
       <c r="C17" s="15" t="s">
         <v>120</v>
       </c>
@@ -6615,7 +6980,7 @@
       <c r="P17" s="3"/>
     </row>
     <row r="18" spans="2:16" ht="63">
-      <c r="B18" s="17"/>
+      <c r="B18" s="19"/>
       <c r="C18" s="7" t="s">
         <v>183</v>
       </c>
@@ -6649,7 +7014,7 @@
       <c r="O18" s="3"/>
     </row>
     <row r="19" spans="2:16" ht="63">
-      <c r="B19" s="17"/>
+      <c r="B19" s="19"/>
       <c r="C19" s="7" t="s">
         <v>174</v>
       </c>
@@ -6689,7 +7054,7 @@
       </c>
     </row>
     <row r="20" spans="2:16" ht="63">
-      <c r="B20" s="17"/>
+      <c r="B20" s="19"/>
       <c r="C20" s="8" t="s">
         <v>186</v>
       </c>
@@ -6725,7 +7090,7 @@
       <c r="O20" s="3"/>
     </row>
     <row r="21" spans="2:16" ht="63">
-      <c r="B21" s="17"/>
+      <c r="B21" s="19"/>
       <c r="C21" s="8" t="s">
         <v>177</v>
       </c>
@@ -6763,7 +7128,7 @@
       <c r="O21" s="3"/>
     </row>
     <row r="22" spans="2:16" ht="63">
-      <c r="B22" s="17"/>
+      <c r="B22" s="19"/>
       <c r="C22" s="7" t="s">
         <v>187</v>
       </c>
@@ -6799,9 +7164,9 @@
       <c r="O22" s="3"/>
     </row>
     <row r="23" spans="2:16" ht="63">
-      <c r="B23" s="17"/>
+      <c r="B23" s="19"/>
       <c r="C23" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D23" t="s">
         <v>3</v>
@@ -6835,7 +7200,7 @@
       <c r="O23" s="3"/>
     </row>
     <row r="24" spans="2:16" ht="63">
-      <c r="B24" s="18" t="s">
+      <c r="B24" s="17" t="s">
         <v>78</v>
       </c>
       <c r="C24" s="7" t="s">
@@ -6871,7 +7236,7 @@
       <c r="O24" s="3"/>
     </row>
     <row r="25" spans="2:16" ht="63">
-      <c r="B25" s="18"/>
+      <c r="B25" s="17"/>
       <c r="C25" s="7" t="s">
         <v>97</v>
       </c>
@@ -6905,126 +7270,194 @@
       <c r="O25" s="3"/>
     </row>
     <row r="26" spans="2:16" ht="63">
-      <c r="B26" s="18"/>
-      <c r="C26" s="7" t="s">
-        <v>190</v>
-      </c>
-      <c r="D26" t="s">
+      <c r="B26" s="17"/>
+      <c r="C26" s="23" t="s">
+        <v>200</v>
+      </c>
+      <c r="D26" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="F26" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="G26" s="16" t="s">
-        <v>153</v>
-      </c>
-      <c r="H26" s="3" t="s">
+      <c r="F26" s="24" t="s">
+        <v>199</v>
+      </c>
+      <c r="G26" s="25" t="s">
+        <v>201</v>
+      </c>
+      <c r="H26" s="21" t="s">
         <v>169</v>
       </c>
-      <c r="I26" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="J26" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="K26" s="3" t="s">
-        <v>53</v>
+      <c r="I26" s="21" t="s">
+        <v>202</v>
+      </c>
+      <c r="J26" s="21" t="s">
+        <v>203</v>
+      </c>
+      <c r="K26" s="21" t="s">
+        <v>93</v>
       </c>
       <c r="L26" s="3"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="6"/>
       <c r="O26" s="3"/>
     </row>
     <row r="27" spans="2:16" ht="63">
-      <c r="B27" s="18"/>
-      <c r="C27" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="D27" t="s">
+      <c r="B27" s="17"/>
+      <c r="C27" s="23" t="s">
+        <v>204</v>
+      </c>
+      <c r="D27" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="F27" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="G27" s="11" t="s">
-        <v>168</v>
-      </c>
-      <c r="H27" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="I27" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="J27" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="K27" s="3" t="s">
-        <v>53</v>
+      <c r="F27" s="24" t="s">
+        <v>198</v>
+      </c>
+      <c r="G27" s="26" t="s">
+        <v>205</v>
+      </c>
+      <c r="H27" s="21" t="s">
+        <v>206</v>
+      </c>
+      <c r="I27" s="21" t="s">
+        <v>202</v>
+      </c>
+      <c r="J27" s="21" t="s">
+        <v>203</v>
+      </c>
+      <c r="K27" s="21" t="s">
+        <v>93</v>
       </c>
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
-      <c r="N27" s="3"/>
+      <c r="N27" s="6"/>
       <c r="O27" s="3"/>
     </row>
-    <row r="28" spans="2:16" ht="42">
-      <c r="B28" s="18"/>
-      <c r="C28" s="9" t="s">
-        <v>194</v>
+    <row r="28" spans="2:16" ht="63">
+      <c r="B28" s="17"/>
+      <c r="C28" s="7" t="s">
+        <v>190</v>
       </c>
       <c r="D28" t="s">
-        <v>61</v>
+        <v>3</v>
       </c>
       <c r="E28" t="s">
-        <v>195</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="G28" s="10" t="s">
-        <v>72</v>
+        <v>4</v>
+      </c>
+      <c r="F28" s="27" t="s">
+        <v>207</v>
+      </c>
+      <c r="G28" s="16" t="s">
+        <v>153</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>198</v>
+        <v>169</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="J28" s="3"/>
+        <v>28</v>
+      </c>
+      <c r="J28" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="K28" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="L28" s="3"/>
       <c r="O28" s="3"/>
     </row>
-    <row r="29" spans="2:16">
-      <c r="C29" s="5"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="6"/>
-      <c r="I29" s="3"/>
+    <row r="29" spans="2:16" ht="63">
+      <c r="B29" s="17"/>
+      <c r="C29" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="D29" t="s">
+        <v>3</v>
+      </c>
+      <c r="E29" t="s">
+        <v>4</v>
+      </c>
+      <c r="F29" s="27" t="s">
+        <v>208</v>
+      </c>
+      <c r="G29" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J29" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="K29" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="L29" s="3"/>
+      <c r="M29" s="3"/>
+      <c r="N29" s="3"/>
+      <c r="O29" s="3"/>
     </row>
-    <row r="35" spans="3:3">
-      <c r="C35" s="5"/>
+    <row r="30" spans="2:16" ht="42">
+      <c r="B30" s="17"/>
+      <c r="C30" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="D30" t="s">
+        <v>61</v>
+      </c>
+      <c r="E30" t="s">
+        <v>194</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="G30" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="J30" s="3"/>
+      <c r="O30" s="3"/>
     </row>
-    <row r="36" spans="3:3">
-      <c r="C36" s="1"/>
+    <row r="31" spans="2:16">
+      <c r="C31" s="5"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="3"/>
+    </row>
+    <row r="37" spans="3:3">
+      <c r="C37" s="5"/>
+    </row>
+    <row r="38" spans="3:3">
+      <c r="C38" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:P28" xr:uid="{DBA4FD5B-D9BE-9A41-89B1-9B1F95EF810F}">
+  <autoFilter ref="A2:P30" xr:uid="{DBA4FD5B-D9BE-9A41-89B1-9B1F95EF810F}">
     <filterColumn colId="1" showButton="0"/>
   </autoFilter>
   <mergeCells count="9">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="B6:B10"/>
+    <mergeCell ref="B11:B15"/>
     <mergeCell ref="O1:O2"/>
     <mergeCell ref="D1:N1"/>
     <mergeCell ref="B1:C2"/>
     <mergeCell ref="B16:B23"/>
-    <mergeCell ref="B24:B28"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="B6:B10"/>
-    <mergeCell ref="B11:B15"/>
+    <mergeCell ref="B24:B30"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7059,40 +7492,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18" t="s">
+      <c r="C1" s="17"/>
+      <c r="D1" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
-      <c r="P1" s="18"/>
-      <c r="Q1" s="18"/>
-      <c r="R1" s="19" t="s">
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="S1" s="18" t="s">
+      <c r="S1" s="17" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:19">
-      <c r="A2" s="19"/>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
+      <c r="A2" s="18"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
       <c r="D2" t="s">
         <v>0</v>
       </c>
@@ -7132,8 +7565,8 @@
       <c r="Q2" t="s">
         <v>22</v>
       </c>
-      <c r="R2" s="19"/>
-      <c r="S2" s="19"/>
+      <c r="R2" s="18"/>
+      <c r="S2" s="18"/>
     </row>
     <row r="3" spans="1:19" ht="42">
       <c r="B3" s="20" t="s">
@@ -7174,7 +7607,7 @@
       </c>
     </row>
     <row r="4" spans="1:19" ht="63">
-      <c r="B4" s="19"/>
+      <c r="B4" s="18"/>
       <c r="C4" s="14" t="s">
         <v>56</v>
       </c>
@@ -7499,7 +7932,7 @@
       <c r="S12" s="3"/>
     </row>
     <row r="13" spans="1:19" ht="63">
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="19" t="s">
         <v>119</v>
       </c>
       <c r="C13" s="13" t="s">
@@ -7543,7 +7976,7 @@
       <c r="S13" s="3"/>
     </row>
     <row r="14" spans="1:19" ht="63">
-      <c r="B14" s="19"/>
+      <c r="B14" s="18"/>
       <c r="C14" s="13" t="s">
         <v>135</v>
       </c>
@@ -7579,7 +8012,7 @@
       <c r="S14" s="3"/>
     </row>
     <row r="15" spans="1:19" ht="63">
-      <c r="B15" s="19"/>
+      <c r="B15" s="18"/>
       <c r="C15" s="13" t="s">
         <v>148</v>
       </c>
@@ -7615,7 +8048,7 @@
       <c r="S15" s="3"/>
     </row>
     <row r="16" spans="1:19" ht="42">
-      <c r="B16" s="19"/>
+      <c r="B16" s="18"/>
       <c r="C16" s="13" t="s">
         <v>136</v>
       </c>
@@ -7651,7 +8084,7 @@
       <c r="S16" s="3"/>
     </row>
     <row r="17" spans="2:20" ht="84">
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="19" t="s">
         <v>95</v>
       </c>
       <c r="C17" s="15" t="s">
@@ -7702,7 +8135,7 @@
       <c r="T17" s="3"/>
     </row>
     <row r="18" spans="2:20" ht="63">
-      <c r="B18" s="17"/>
+      <c r="B18" s="19"/>
       <c r="C18" s="7" t="s">
         <v>89</v>
       </c>
@@ -7741,7 +8174,7 @@
       </c>
     </row>
     <row r="19" spans="2:20" ht="63">
-      <c r="B19" s="17"/>
+      <c r="B19" s="19"/>
       <c r="C19" s="4" t="s">
         <v>39</v>
       </c>
@@ -7776,7 +8209,7 @@
       <c r="R19" s="3"/>
     </row>
     <row r="20" spans="2:20" ht="63">
-      <c r="B20" s="17"/>
+      <c r="B20" s="19"/>
       <c r="C20" s="8" t="s">
         <v>80</v>
       </c>
@@ -7815,7 +8248,7 @@
       </c>
     </row>
     <row r="21" spans="2:20" ht="63">
-      <c r="B21" s="17"/>
+      <c r="B21" s="19"/>
       <c r="C21" s="4" t="s">
         <v>40</v>
       </c>
@@ -7850,7 +8283,7 @@
       <c r="R21" s="3"/>
     </row>
     <row r="22" spans="2:20" ht="63">
-      <c r="B22" s="17"/>
+      <c r="B22" s="19"/>
       <c r="C22" s="7" t="s">
         <v>81</v>
       </c>
@@ -7885,7 +8318,7 @@
       <c r="R22" s="3"/>
     </row>
     <row r="23" spans="2:20" ht="63">
-      <c r="B23" s="18" t="s">
+      <c r="B23" s="17" t="s">
         <v>78</v>
       </c>
       <c r="C23" s="7" t="s">
@@ -7922,7 +8355,7 @@
       </c>
     </row>
     <row r="24" spans="2:20" ht="63">
-      <c r="B24" s="18"/>
+      <c r="B24" s="17"/>
       <c r="C24" s="7" t="s">
         <v>94</v>
       </c>
@@ -7954,7 +8387,7 @@
       </c>
     </row>
     <row r="25" spans="2:20" ht="63">
-      <c r="B25" s="18"/>
+      <c r="B25" s="17"/>
       <c r="C25" s="9" t="s">
         <v>74</v>
       </c>
@@ -7990,7 +8423,7 @@
       <c r="S25" s="3"/>
     </row>
     <row r="26" spans="2:20" ht="63">
-      <c r="B26" s="18"/>
+      <c r="B26" s="17"/>
       <c r="C26" s="1" t="s">
         <v>45</v>
       </c>
@@ -8018,7 +8451,7 @@
       <c r="R26" s="3"/>
     </row>
     <row r="27" spans="2:20" ht="63">
-      <c r="B27" s="18"/>
+      <c r="B27" s="17"/>
       <c r="C27" s="1" t="s">
         <v>25</v>
       </c>
@@ -8046,7 +8479,7 @@
       <c r="R27" s="3"/>
     </row>
     <row r="28" spans="2:20" ht="63">
-      <c r="B28" s="18"/>
+      <c r="B28" s="17"/>
       <c r="C28" s="5" t="s">
         <v>24</v>
       </c>
@@ -8074,7 +8507,7 @@
       <c r="R28" s="3"/>
     </row>
     <row r="29" spans="2:20" ht="63">
-      <c r="B29" s="19" t="s">
+      <c r="B29" s="18" t="s">
         <v>99</v>
       </c>
       <c r="C29" s="4" t="s">
@@ -8109,7 +8542,7 @@
       <c r="R29" s="3"/>
     </row>
     <row r="30" spans="2:20" ht="84">
-      <c r="B30" s="19"/>
+      <c r="B30" s="18"/>
       <c r="C30" s="5" t="s">
         <v>48</v>
       </c>
@@ -8149,17 +8582,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:C2"/>
-    <mergeCell ref="D1:Q1"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="B29:B30"/>
     <mergeCell ref="S1:S2"/>
     <mergeCell ref="B5:B12"/>
     <mergeCell ref="B13:B16"/>
     <mergeCell ref="B17:B22"/>
     <mergeCell ref="B23:B28"/>
     <mergeCell ref="B3:B4"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:C2"/>
+    <mergeCell ref="D1:Q1"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="B29:B30"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>